<commit_message>
JdT et rapport - Bryan
</commit_message>
<xml_diff>
--- a/Doc/JournauxTravail/Journal_Travail_Bryan.xlsx
+++ b/Doc/JournauxTravail/Journal_Travail_Bryan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{02A813EF-7570-433A-95A5-26520B3E63E5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B17C299C-26DE-4AE3-811A-48B0EF733B5F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10800" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12000" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>Vac</t>
+  </si>
+  <si>
+    <t>Elaboration de la vue de la liste des budgets, premier essais du formulaire des budget</t>
+  </si>
+  <si>
+    <t>Implémentation de la suppression et de la modification d'un objet</t>
+  </si>
+  <si>
+    <t>Utilisation des méthode de modification et de suppression dans la DB, implémentation da la partie confirmation de l'enregistrement</t>
+  </si>
+  <si>
+    <t>Revue de la structure de certaines fenêtres, élaboration de certains détails. Documentation (JdT, rapport)</t>
   </si>
 </sst>
 </file>
@@ -220,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -486,11 +498,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -549,53 +576,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,28 +926,28 @@
       <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:5" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:5" s="27" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -931,11 +961,11 @@
       <c r="C5" s="15">
         <v>0.25</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="34">
         <f>SUM(C5:C6)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="32">
         <v>1</v>
       </c>
     </row>
@@ -949,8 +979,8 @@
       <c r="C6" s="16">
         <v>0.75</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="29"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -962,11 +992,11 @@
       <c r="C7" s="17">
         <v>0.5</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="36">
         <f>SUM(C7:C11)</f>
         <v>12</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>2</v>
       </c>
     </row>
@@ -980,8 +1010,8 @@
       <c r="C8" s="15">
         <v>1</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="31"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -993,8 +1023,8 @@
       <c r="C9" s="15">
         <v>2</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -1006,8 +1036,8 @@
       <c r="C10" s="15">
         <v>4.75</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="31"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
@@ -1019,8 +1049,8 @@
       <c r="C11" s="16">
         <v>3.75</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="29"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -1032,11 +1062,11 @@
       <c r="C12" s="17">
         <v>2</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="36">
         <f>SUM(C12:C16)</f>
         <v>7.75</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>3</v>
       </c>
     </row>
@@ -1050,8 +1080,8 @@
       <c r="C13" s="15">
         <v>1.5</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="31"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -1063,8 +1093,8 @@
       <c r="C14" s="15">
         <v>1</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="31"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="30"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -1076,8 +1106,8 @@
       <c r="C15" s="15">
         <v>1.25</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="31"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
@@ -1089,8 +1119,8 @@
       <c r="C16" s="16">
         <v>2</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="29"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -1102,11 +1132,11 @@
       <c r="C17" s="17">
         <v>0.5</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="36">
         <f>SUM(C17:C19)</f>
         <v>3.5</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="29">
         <v>4</v>
       </c>
     </row>
@@ -1120,8 +1150,8 @@
       <c r="C18" s="15">
         <v>1</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="31"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="30"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
@@ -1133,8 +1163,8 @@
       <c r="C19" s="16">
         <v>2</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="29"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
@@ -1146,11 +1176,11 @@
       <c r="C20" s="17">
         <v>1.5</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="36">
         <f>SUM(C20:C23)</f>
         <v>7.45</v>
       </c>
-      <c r="E20" s="30">
+      <c r="E20" s="29">
         <v>5</v>
       </c>
     </row>
@@ -1164,8 +1194,8 @@
       <c r="C21" s="17">
         <v>1</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="31"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="30"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -1177,8 +1207,8 @@
       <c r="C22" s="15">
         <v>2.5</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="31"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
@@ -1190,8 +1220,8 @@
       <c r="C23" s="16">
         <v>2.4500000000000002</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="31"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
@@ -1203,11 +1233,11 @@
       <c r="C24" s="17">
         <v>1.5</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="37">
         <f>SUM(C24:C26)</f>
         <v>3.75</v>
       </c>
-      <c r="E24" s="30">
+      <c r="E24" s="29">
         <v>6</v>
       </c>
     </row>
@@ -1221,8 +1251,8 @@
       <c r="C25" s="15">
         <v>1.25</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="31"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="30"/>
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
@@ -1234,8 +1264,8 @@
       <c r="C26" s="16">
         <v>1</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="29"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -1247,11 +1277,11 @@
       <c r="C27" s="17">
         <v>0.75</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="36">
         <f>SUM(C27:C28)</f>
         <v>2.5</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="29" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1265,8 +1295,8 @@
       <c r="C28" s="16">
         <v>1.75</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="29"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
@@ -1278,11 +1308,11 @@
       <c r="C29" s="17">
         <v>1.5</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="36">
         <f>SUM(C29:C33)</f>
         <v>11</v>
       </c>
-      <c r="E29" s="30">
+      <c r="E29" s="29">
         <v>7</v>
       </c>
     </row>
@@ -1296,8 +1326,8 @@
       <c r="C30" s="15">
         <v>2</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="31"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="30"/>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -1309,8 +1339,8 @@
       <c r="C31" s="15">
         <v>2</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="31"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -1322,8 +1352,8 @@
       <c r="C32" s="15">
         <v>4</v>
       </c>
-      <c r="D32" s="23"/>
-      <c r="E32" s="31"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="30"/>
     </row>
     <row r="33" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
@@ -1335,8 +1365,8 @@
       <c r="C33" s="16">
         <v>1.5</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="29"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
@@ -1348,11 +1378,11 @@
       <c r="C34" s="21">
         <v>0.25</v>
       </c>
-      <c r="D34" s="22">
+      <c r="D34" s="36">
         <f>SUM(C34:C35)</f>
         <v>1.25</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="29">
         <v>8</v>
       </c>
     </row>
@@ -1366,8 +1396,8 @@
       <c r="C35" s="16">
         <v>1</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="29"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
@@ -1379,11 +1409,11 @@
       <c r="C36" s="21">
         <v>1.5</v>
       </c>
-      <c r="D36" s="22">
+      <c r="D36" s="36">
         <f>SUM(C36:C37)</f>
         <v>6.5</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="29">
         <v>9</v>
       </c>
     </row>
@@ -1397,74 +1427,107 @@
       <c r="C37" s="16">
         <v>5</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="29"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="18">
         <v>43220</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="21">
         <v>1.5</v>
       </c>
-      <c r="D38" s="27"/>
+      <c r="D38" s="36">
+        <f>SUM(C38:C41)</f>
+        <v>12.75</v>
+      </c>
+      <c r="E38" s="36">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="38">
         <v>43221</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="15">
         <v>3.25</v>
       </c>
-      <c r="D39" s="27"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="27"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="27"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="27"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="27"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="38">
+        <v>43232</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="15">
+        <v>3</v>
+      </c>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+    </row>
+    <row r="41" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20">
+        <v>43226</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="16">
+        <v>5</v>
+      </c>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>43227</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="10">
+        <v>3</v>
+      </c>
+      <c r="D42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43228</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="6">
+        <v>3</v>
+      </c>
+      <c r="D43" s="22"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="27"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="27"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="27"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
@@ -1472,12 +1535,14 @@
       </c>
       <c r="C47" s="7">
         <f>SUM(C5:C46)</f>
-        <v>61.45</v>
-      </c>
-      <c r="D47" s="37"/>
+        <v>75.45</v>
+      </c>
+      <c r="D47" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
+    <mergeCell ref="D38:D41"/>
+    <mergeCell ref="E38:E41"/>
     <mergeCell ref="D27:D28"/>
     <mergeCell ref="D29:D33"/>
     <mergeCell ref="D34:D35"/>

</xml_diff>